<commit_message>
quick fix on OM
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76D370F-7120-ED4C-9C86-CE2042039FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0F3010-BEB1-DD4D-8765-074746E70E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="740" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="5" r:id="rId1"/>
@@ -981,7 +981,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1046,7 +1046,7 @@
         <v>35</v>
       </c>
       <c r="B6">
-        <v>9.8485999999999994</v>
+        <v>6.1</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
pushing recent version of EM - BH unbiased for pollock.
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0F3010-BEB1-DD4D-8765-074746E70E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72318EC8-0204-FC4E-8354-95C32F7E4B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
+    <workbookView xWindow="5040" yWindow="600" windowWidth="30240" windowHeight="18880" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="5" r:id="rId1"/>
@@ -534,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8369A2B-907E-A04C-AB33-D4BAA4CA0759}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -556,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68234D63-F072-F546-83AF-F96BE681F2D5}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1024,7 +1024,7 @@
         <v>32</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
finishing up some runs... but should be decent w/ recruitment?
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72318EC8-0204-FC4E-8354-95C32F7E4B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5B71E4-64ED-8B41-B4A0-11781A4DB978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="600" windowWidth="30240" windowHeight="18880" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="5" r:id="rId1"/>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8369A2B-907E-A04C-AB33-D4BAA4CA0759}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -980,7 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68234D63-F072-F546-83AF-F96BE681F2D5}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1024,7 +1024,7 @@
         <v>32</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
reordering idnexing in the OM
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F80D70-F84B-5240-9570-D4AE54498ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CA8B9A-9A85-5040-9398-274167690CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>
@@ -579,7 +579,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>10000000</v>
+        <v>300</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -726,7 +726,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:R1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E2">
         <v>8.0000000000000002E-3</v>
@@ -982,7 +982,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,7 +1025,7 @@
         <v>32</v>
       </c>
       <c r="B4">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
sablefish needs to be run longer to reach unfished state
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CA8B9A-9A85-5040-9398-274167690CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB450F24-859A-6B40-9339-7457B756AB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
OM EM has been fixed!
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB450F24-859A-6B40-9339-7457B756AB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFD6E17-472B-3C4B-90FF-1B7762298268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="5" r:id="rId1"/>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8369A2B-907E-A04C-AB33-D4BAA4CA0759}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -981,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68234D63-F072-F546-83AF-F96BE681F2D5}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1025,7 +1025,7 @@
         <v>32</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
implementing saturating version of DM
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFD6E17-472B-3C4B-90FF-1B7762298268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C594E4B-06C2-6F4E-8155-FEC640064700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="5" r:id="rId1"/>
@@ -535,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8369A2B-907E-A04C-AB33-D4BAA4CA0759}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>
@@ -568,7 +568,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -579,7 +579,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -981,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68234D63-F072-F546-83AF-F96BE681F2D5}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating time-varying selex options
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C594E4B-06C2-6F4E-8155-FEC640064700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78211F5B-B673-6946-9EEB-2020B06BF01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
adding documentation to simulate_data function
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78211F5B-B673-6946-9EEB-2020B06BF01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E93FC7E-099C-DF4A-8D2A-BC012583EB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
add in f-based spr calcs
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1575C7-66AD-A64F-95DC-867DFB0A19FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7530ABCC-DAB3-A54F-B1F1-E97F60A0D584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="5" r:id="rId1"/>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8369A2B-907E-A04C-AB33-D4BAA4CA0759}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>
@@ -601,7 +601,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -981,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68234D63-F072-F546-83AF-F96BE681F2D5}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
quick fixes and tests - simulations should be good to go
</commit_message>
<xml_diff>
--- a/input/EBS_Pollock_Inputs.xlsx
+++ b/input/EBS_Pollock_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7530ABCC-DAB3-A54F-B1F1-E97F60A0D584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9463D9-D60B-8141-A36B-632FC91E8051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{B9FAFB83-B8A9-0040-835E-CA2E963D682F}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -982,7 +982,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,7 +1025,7 @@
         <v>32</v>
       </c>
       <c r="B4">
-        <v>0.01</v>
+        <v>0.8</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>

</xml_diff>